<commit_message>
Adicioinar 'PF por Funcionalidade' em todos os relatórios e planilhas - BASIS-235322
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="Lista" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Estórias " sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Regras" sheetId="8" state="hidden" r:id="rId9"/>
+    <sheet name="PF por Funcionalidade" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Lista!$A$2:$E$33</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="201">
   <si>
     <t xml:space="preserve">Chamado [Número] - [Sigla do Sistema]</t>
   </si>
@@ -657,6 +658,15 @@
   <si>
     <t xml:space="preserve">SISP</t>
   </si>
+  <si>
+    <t xml:space="preserve">Nº</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcionalidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF Ajust.</t>
+  </si>
 </sst>
 </file>
 
@@ -664,16 +674,16 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="D/MMM"/>
-    <numFmt numFmtId="167" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="D/MMM"/>
+    <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.00%"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.00"/>
     <numFmt numFmtId="172" formatCode="0"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="54">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -695,12 +705,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -924,6 +928,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1036,6 +1046,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1105,7 +1127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1162,8 +1184,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1188,398 +1217,387 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="175">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="5" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="5" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="17" fillId="6" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="16" fillId="6" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="17" fillId="6" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="16" fillId="6" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="33" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="172" fontId="33" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="171" fontId="35" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -1607,11 +1625,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1631,27 +1649,27 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1699,19 +1717,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1867,48 +1885,57 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="31" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="30" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="33" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="52" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 7" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Porcentagem 2" xfId="23" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="269">
+  <dxfs count="267">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -3508,19 +3535,6 @@
         <color rgb="FF000000"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Cambria"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF0066FF"/>
-      </font>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -3596,7 +3610,7 @@
   </sheetPr>
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3899,7 +3913,7 @@
   </sheetPr>
   <dimension ref="B1:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -3912,7 +3926,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="24"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="15" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="15" width="9.14"/>
@@ -4818,7 +4832,7 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4839,7 +4853,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="69" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="69" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="15" style="64" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="249" style="64" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="249" style="64" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="251" min="251" style="64" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="252" style="64" width="9.14"/>
   </cols>
@@ -5349,7 +5363,7 @@
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.920138888888889" bottom="0.7875" header="0.315277777777778" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.920138888888889" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5366,7 +5380,7 @@
   </sheetPr>
   <dimension ref="A1:AK203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -5378,32 +5392,32 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="112" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="112" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="112" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="112" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="112" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="112" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="112" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="112" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="112" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="112" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="112" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="112" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="112" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="113" width="8"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="113" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="113" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="113" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="113" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="114" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="113" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="114" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="115" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="116" width="1.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="117" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="112" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="112" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="112" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="112" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="112" width="4.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="112" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="113" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="113" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="113" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="113" width="4"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="113" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="113" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="118" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="31" style="118" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="119" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="116" width="1.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="119" width="34"/>
@@ -23816,975 +23830,975 @@
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y3:Y4">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:X3 U6:X6 X7 U9:X12 W8:X8">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A9">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106:B202 B4:B88 B92:B102">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R88 R92:R97">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3:AH98">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AJ97">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK23 AK25 AK5 AK28:AK91">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>ISBLANK($R5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
       <formula>$R5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
       <formula>$I5&lt;&gt;$Y5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98 G98 E98">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98 D100:D101">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:E99 G99">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R98">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>ISBLANK($R98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
       <formula>$R98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
       <formula>$I98&lt;&gt;$Y98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F92:F101">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>ISBLANK($T92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
       <formula>$T92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>$K92&lt;&gt;$AA92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105 E105 G105:H105">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103 G103 E103">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103 D105">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104:E104 G104">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H104">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103:F105">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R103">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
+    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R104">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
       <formula>ISBLANK($R104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
       <formula>$R104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
+    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>$I104&lt;&gt;$Y104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R99:R101">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91 E91 G91:H91">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89 G89 E89">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89 D91">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:E90 G90">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89:F91">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R91">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R89">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
       <formula>ISBLANK($R89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
       <formula>$R89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
       <formula>$I89&lt;&gt;$Y89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R90">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
       <formula>ISBLANK($R90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
       <formula>$R90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
       <formula>$I90&lt;&gt;$Y90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:X4">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
+    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:X5">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH103">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:W7">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
       <formula>ISBLANK($T7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
       <formula>$T7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
       <formula>$K7&lt;&gt;$AA7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13:X13">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
+    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
+    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14:X14">
-    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15:X15">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:X16">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:W101 U30:W39 U41:W88 W40">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U98 W98">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
+    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V98 V100:V101">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
+    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U99:W99">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W91">
-    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
+    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W89">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
+    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W90">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30:X88 X92:X101">
-    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
+    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
+    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X98">
-    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X99">
-    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X91">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X89">
-    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
+    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X90">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
+    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH99:AH101">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
       <formula>ISBLANK($R6)</formula>
     </cfRule>
-    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
       <formula>$R6="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
+    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
       <formula>$I6&lt;&gt;$Y6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T89:T91">
-    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
+    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
+    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U89:V91">
-    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
+    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
+    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK26:AK27">
-    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
+    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
       <formula>ISBLANK($R26)</formula>
     </cfRule>
-    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
+    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
       <formula>$R26="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
+    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
       <formula>$I26&lt;&gt;$Y26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK24">
-    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
+    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
       <formula>ISBLANK($R24)</formula>
     </cfRule>
-    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
+    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
       <formula>$R24="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
       <formula>$I24&lt;&gt;$Y24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK22">
-    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
+    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
       <formula>ISBLANK($R9)</formula>
     </cfRule>
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
       <formula>$R9="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
+    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
       <formula>$I9&lt;&gt;$Y9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK7">
-    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
+    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
       <formula>ISBLANK($R7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
       <formula>$R7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
+    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
       <formula>$I7&lt;&gt;$Y7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
+    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
       <formula>ISBLANK($R4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
       <formula>$R4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
+    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
       <formula>$I4&lt;&gt;$Y4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK3">
-    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
+    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
+    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK92:AK101">
-    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
+    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
       <formula>ISBLANK($R92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
+    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
       <formula>$R92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
       <formula>$I92&lt;&gt;$Y92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
       <formula>ISBLANK($R8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
+    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
       <formula>$R8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
+    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
       <formula>$I8&lt;&gt;$Y8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U40:V40">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
       <formula>ISBLANK($T40)</formula>
     </cfRule>
-    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
+    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
       <formula>$T40="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263">
+    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
       <formula>$K40&lt;&gt;$AA40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:V8">
-    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264">
+    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
       <formula>ISBLANK($T8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="265">
+    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263">
       <formula>$T8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="266">
+    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264">
       <formula>$K8&lt;&gt;$AA8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24827,7 +24841,7 @@
   </sheetPr>
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -25386,7 +25400,7 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -26015,7 +26029,7 @@
   </sheetPr>
   <dimension ref="B2:C99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -26733,13 +26747,13 @@
   </sheetPr>
   <dimension ref="A4:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="171" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
@@ -26768,4 +26782,225 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="172" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="172" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="172" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="173"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="173"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="174"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="174"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="173"/>
+      <c r="B6" s="174"/>
+      <c r="C6" s="174"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="173"/>
+      <c r="B7" s="174"/>
+      <c r="C7" s="174"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="173"/>
+      <c r="B8" s="174"/>
+      <c r="C8" s="174"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="173"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
+      <c r="C10" s="174"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
+      <c r="C11" s="174"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
+      <c r="C12" s="174"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="173"/>
+      <c r="B13" s="174"/>
+      <c r="C13" s="174"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="173"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="173"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="174"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="173"/>
+      <c r="B16" s="174"/>
+      <c r="C16" s="174"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="173"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="174"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="173"/>
+      <c r="B18" s="174"/>
+      <c r="C18" s="174"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="173"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="173"/>
+      <c r="B20" s="174"/>
+      <c r="C20" s="174"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="173"/>
+      <c r="B21" s="174"/>
+      <c r="C21" s="174"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="173"/>
+      <c r="B22" s="174"/>
+      <c r="C22" s="174"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="173"/>
+      <c r="B23" s="174"/>
+      <c r="C23" s="174"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="173"/>
+      <c r="B24" s="174"/>
+      <c r="C24" s="174"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="173"/>
+      <c r="B25" s="174"/>
+      <c r="C25" s="174"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="173"/>
+      <c r="B26" s="174"/>
+      <c r="C26" s="174"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="173"/>
+      <c r="B27" s="174"/>
+      <c r="C27" s="174"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="173"/>
+      <c r="B28" s="174"/>
+      <c r="C28" s="174"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="173"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="174"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="173"/>
+      <c r="B30" s="174"/>
+      <c r="C30" s="174"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="173"/>
+      <c r="B31" s="174"/>
+      <c r="C31" s="174"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="173"/>
+      <c r="B32" s="174"/>
+      <c r="C32" s="174"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="173"/>
+      <c r="B33" s="174"/>
+      <c r="C33" s="174"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="173"/>
+      <c r="B34" s="174"/>
+      <c r="C34" s="174"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="173"/>
+      <c r="B35" s="174"/>
+      <c r="C35" s="174"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="173"/>
+      <c r="B36" s="174"/>
+      <c r="C36" s="174"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="173"/>
+      <c r="B37" s="174"/>
+      <c r="C37" s="174"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustar planilhas e erro do PDF - BASIS-235322
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
+++ b/backend/src/main/resources/reports/planilhas/modelo3-anac.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revisão" sheetId="1" state="visible" r:id="rId2"/>
@@ -1935,7 +1935,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="267">
+  <dxfs count="265">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -3522,19 +3522,6 @@
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <name val="Cambria"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF0066FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -3913,7 +3900,7 @@
   </sheetPr>
   <dimension ref="B1:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4507,7 +4494,7 @@
     <row r="39" s="53" customFormat="true" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="54" t="str">
         <f aca="false">CONCATENATE(B24,":",D24*100,"%")</f>
-        <v>    % de Divergência:0%</v>
+        <v>% de Divergência:0%</v>
       </c>
       <c r="C39" s="54"/>
       <c r="D39" s="54"/>
@@ -23838,967 +23825,967 @@
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:X3 U6:X6 X7 U9:X12 W8:X8">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A9">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106:B202 B4:B88 B92:B102">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>ISBLANK($T3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>$T3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>$K3&lt;&gt;$AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R88 R92:R97">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3:AH98">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AJ97">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK23 AK25 AK5 AK28:AK91">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>ISBLANK($R5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>$R5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
       <formula>$I5&lt;&gt;$Y5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98 G98 E98">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98 D100:D101">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:E99 G99">
-    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R98">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
       <formula>ISBLANK($R98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>$R98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>$I98&lt;&gt;$Y98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F92:F101">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
       <formula>ISBLANK($T92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
       <formula>$T92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>$K92&lt;&gt;$AA92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105 E105 G105:H105">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103 G103 E103">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103 D105">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104:E104 G104">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B104">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H104">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
+    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
       <formula>ISBLANK($T104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
       <formula>$T104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>$K104&lt;&gt;$AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103:F105">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
       <formula>ISBLANK($T103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
       <formula>$T103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
       <formula>$K103&lt;&gt;$AA103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R105">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>ISBLANK($T105)</formula>
     </cfRule>
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>$T105="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>$K105&lt;&gt;$AA105</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R103">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R104">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
       <formula>ISBLANK($R104)</formula>
     </cfRule>
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>$R104="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
       <formula>$I104&lt;&gt;$Y104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R99:R101">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91 E91 G91:H91">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
+    <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89 G89 E89">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
+    <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
+    <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
+    <cfRule type="expression" priority="119" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89 D91">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
+    <cfRule type="expression" priority="123" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:E90 G90">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
+    <cfRule type="expression" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
+    <cfRule type="expression" priority="130" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
+    <cfRule type="expression" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89:F91">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
+    <cfRule type="expression" priority="136" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R91">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R89">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
       <formula>ISBLANK($R89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
       <formula>$R89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
+    <cfRule type="expression" priority="142" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
       <formula>$I89&lt;&gt;$Y89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R90">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
       <formula>ISBLANK($R90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
+    <cfRule type="expression" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
       <formula>$R90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
       <formula>$I90&lt;&gt;$Y90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
+    <cfRule type="expression" priority="147" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:X4">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
       <formula>ISBLANK($T4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
+    <cfRule type="expression" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
       <formula>$T4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
+    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
       <formula>$K4&lt;&gt;$AA4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
+    <cfRule type="expression" priority="153" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:X5">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
       <formula>ISBLANK($T5)</formula>
     </cfRule>
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
       <formula>$T5="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
       <formula>$K5&lt;&gt;$AA5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH103">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
       <formula>ISBLANK($R103)</formula>
     </cfRule>
-    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
+    <cfRule type="expression" priority="159" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
       <formula>$R103="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
       <formula>$I103&lt;&gt;$Y103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:W7">
-    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
+    <cfRule type="expression" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
       <formula>ISBLANK($T7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
       <formula>$T7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
       <formula>$K7&lt;&gt;$AA7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13">
-    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="expression" priority="164" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U13:X13">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
       <formula>ISBLANK($T13)</formula>
     </cfRule>
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
       <formula>$T13="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
+    <cfRule type="expression" priority="169" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
       <formula>$K13&lt;&gt;$AA13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
+    <cfRule type="expression" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14:X14">
-    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
       <formula>ISBLANK($T14)</formula>
     </cfRule>
-    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
+    <cfRule type="expression" priority="174" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
       <formula>$T14="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
       <formula>$K14&lt;&gt;$AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
+    <cfRule type="expression" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="172">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15:X15">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="173">
       <formula>ISBLANK($T15)</formula>
     </cfRule>
-    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
+    <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="174">
       <formula>$T15="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="175">
       <formula>$K15&lt;&gt;$AA15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="176">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
+    <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:X16">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
       <formula>ISBLANK($T16)</formula>
     </cfRule>
-    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
+    <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
       <formula>$T16="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
       <formula>$K16&lt;&gt;$AA16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:W101 U30:W39 U41:W88 W40">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
+    <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U98 W98">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
+    <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
+    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V98 V100:V101">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
+    <cfRule type="expression" priority="195" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U99:W99">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="191">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="192">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="193">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W91">
-    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
+    <cfRule type="expression" priority="200" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="194">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="195">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
+    <cfRule type="expression" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="196">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W89">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="197">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="198">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
+    <cfRule type="expression" priority="205" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="199">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W90">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="200">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="201">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="202">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30:X88 X92:X101">
-    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
+    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="203">
       <formula>ISBLANK($T30)</formula>
     </cfRule>
-    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
+    <cfRule type="expression" priority="210" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="204">
       <formula>$T30="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="205">
       <formula>$K30&lt;&gt;$AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X98">
-    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
+    <cfRule type="expression" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="206">
       <formula>ISBLANK($T98)</formula>
     </cfRule>
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="207">
       <formula>$T98="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="208">
       <formula>$K98&lt;&gt;$AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X99">
-    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
+    <cfRule type="expression" priority="215" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="209">
       <formula>ISBLANK($T99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="210">
       <formula>$T99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="211">
       <formula>$K99&lt;&gt;$AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X91">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="212">
       <formula>ISBLANK($T91)</formula>
     </cfRule>
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="213">
       <formula>$T91="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="214">
       <formula>$K91&lt;&gt;$AA91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X89">
-    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
+    <cfRule type="expression" priority="221" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="215">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="216">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
+    <cfRule type="expression" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="217">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X90">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="218">
       <formula>ISBLANK($T90)</formula>
     </cfRule>
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="219">
       <formula>$T90="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
+    <cfRule type="expression" priority="226" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="220">
       <formula>$K90&lt;&gt;$AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH99:AH101">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="221">
       <formula>ISBLANK($R99)</formula>
     </cfRule>
-    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="222">
       <formula>$R99="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="223">
       <formula>$I99&lt;&gt;$Y99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="224">
       <formula>ISBLANK($R6)</formula>
     </cfRule>
-    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
+    <cfRule type="expression" priority="231" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="225">
       <formula>$R6="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
+    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="226">
       <formula>$I6&lt;&gt;$Y6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T89:T91">
-    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
+    <cfRule type="expression" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="227">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="228">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
+    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U89:V91">
-    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
+    <cfRule type="expression" priority="236" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="230">
       <formula>ISBLANK($T89)</formula>
     </cfRule>
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="231">
       <formula>$T89="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
+    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="232">
       <formula>$K89&lt;&gt;$AA89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK26:AK27">
-    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
+    <cfRule type="expression" priority="239" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="233">
       <formula>ISBLANK($R26)</formula>
     </cfRule>
-    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
+    <cfRule type="expression" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="234">
       <formula>$R26="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
+    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="235">
       <formula>$I26&lt;&gt;$Y26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK24">
-    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
+    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="236">
       <formula>ISBLANK($R24)</formula>
     </cfRule>
-    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
+    <cfRule type="expression" priority="243" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="237">
       <formula>$R24="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="238">
       <formula>$I24&lt;&gt;$Y24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK22">
-    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
+    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="239">
       <formula>ISBLANK($R9)</formula>
     </cfRule>
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="240">
       <formula>$R9="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
+    <cfRule type="expression" priority="247" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="241">
       <formula>$I9&lt;&gt;$Y9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK7">
-    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
+    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="242">
       <formula>ISBLANK($R7)</formula>
     </cfRule>
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="243">
       <formula>$R7="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
+    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="244">
       <formula>$I7&lt;&gt;$Y7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
+    <cfRule type="expression" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="245">
       <formula>ISBLANK($R4)</formula>
     </cfRule>
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="246">
       <formula>$R4="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
+    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="247">
       <formula>$I4&lt;&gt;$Y4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK3">
-    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
+    <cfRule type="expression" priority="254" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="248">
       <formula>ISBLANK($R3)</formula>
     </cfRule>
-    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
+    <cfRule type="expression" priority="255" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="249">
       <formula>$R3="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="250">
       <formula>$I3&lt;&gt;$Y3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK92:AK101">
-    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
+    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="251">
       <formula>ISBLANK($R92)</formula>
     </cfRule>
-    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
+    <cfRule type="expression" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="252">
       <formula>$R92="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="253">
       <formula>$I92&lt;&gt;$Y92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="254">
       <formula>ISBLANK($R8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
+    <cfRule type="expression" priority="261" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="255">
       <formula>$R8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
+    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="256">
       <formula>$I8&lt;&gt;$Y8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U40:V40">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="257">
       <formula>ISBLANK($T40)</formula>
     </cfRule>
-    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
+    <cfRule type="expression" priority="264" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="258">
       <formula>$T40="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
+    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="259">
       <formula>$K40&lt;&gt;$AA40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:V8">
-    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
+    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="260">
       <formula>ISBLANK($T8)</formula>
     </cfRule>
-    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="263">
+    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="261">
       <formula>$T8="NOK"</formula>
     </cfRule>
-    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="264">
+    <cfRule type="expression" priority="268" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="262">
       <formula>$K8&lt;&gt;$AA8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26791,7 +26778,7 @@
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>